<commit_message>
Updated functions and removed scores for CS, CW, and Connection to Place for only presenting draft framework with modified goals
</commit_message>
<xml_diff>
--- a/status and goal table.xlsx
+++ b/status and goal table.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="228">
   <si>
     <t>Hawaii Ocean Health Index Draft Framework</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>Fishponds</t>
-  </si>
-  <si>
-    <t># active and/or undergoing restoration</t>
   </si>
   <si>
     <t xml:space="preserve">Loko ia and OHA </t>
@@ -493,27 +490,6 @@
     <t>IUCN</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Habitats: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">The extent, condition, and level of protection of coastal and terrestrial habitats, recognizing that connection between land and sea for maintaining a healthy ocean. Habitat that have specific linked management initiatives are factored into their score. If no management action in set in place then a penalty may be applied based on stakeholder recommendations. </t>
-    </r>
-  </si>
-  <si>
     <t>The extent, condition, and level of protection of coastal and terrestrial habitats, recognizing that connection between land and sea for maintaining a healthy ocean.</t>
   </si>
   <si>
@@ -736,9 +712,6 @@
     <t>USDA available:https://quickstats.nass.usda.gov/</t>
   </si>
   <si>
-    <t>sustainability risk assessment scaled from 0-1 based on biosecurity threat, invasive species threat, and feed type (protien vs. plant)</t>
-  </si>
-  <si>
     <t>DAR species list</t>
   </si>
   <si>
@@ -820,9 +793,6 @@
     <t>lbs produced estimated to county by ratio of opperators per county for finfish and shellfish</t>
   </si>
   <si>
-    <t>USFWS National Wetlands Inventory clipped to 1km of the coast and deepwater habitats removed</t>
-  </si>
-  <si>
     <t>NOAA ESI and Fletcher et al 2012 (https://pubs.usgs.gov/of/2011/1051/pdf/ofr2011-1051_report_508.pdf)</t>
   </si>
   <si>
@@ -859,9 +829,6 @@
     <t>Reference Point TBD</t>
   </si>
   <si>
-    <t>Lasting Special Places</t>
-  </si>
-  <si>
     <t>Marine Managed Areas</t>
   </si>
   <si>
@@ -898,9 +865,6 @@
     <t>Nutrient models</t>
   </si>
   <si>
-    <t>Connection to Place</t>
-  </si>
-  <si>
     <t xml:space="preserve">Zero beach closures and/or levels that do not exceed closure levels or proxy is # of cesspools </t>
   </si>
   <si>
@@ -947,13 +911,86 @@
   </si>
   <si>
     <t xml:space="preserve">Number of impaired coastal waters/target number of improved coastal waters </t>
+  </si>
+  <si>
+    <t>sustainability risk assessment scaled from 0-1 based on biosecurity threat, invasive species threat, and feed type (protein vs. plant)</t>
+  </si>
+  <si>
+    <t>30% of historical fishponds are active or undergoing restoration</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Habitats: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>The extent, condition, and level of protection of coastal and terrestrial habitats, recognizing that connection between land and sea for maintaining a healthy ocean.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lasting Special Places: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>The protection of marine and coastal areas and sacred and historical sites.</t>
+    </r>
+  </si>
+  <si>
+    <t>NOAA MPA Inventory</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Connection to Place: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> The connection that people have to coastal and marine environments.</t>
+    </r>
+  </si>
+  <si>
+    <t>Carbon Storage</t>
+  </si>
+  <si>
+    <t>The extent and condition of coastal habitats (wetlands) that offer long term (&gt;100yrs) carbon storage.</t>
+  </si>
+  <si>
+    <t>NOAA CCAP wetlands clipped to 1km of coastline</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>Contact: Eva Schemmel, Conservation International Hawaii, eschemmel@conservation.org</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1051,10 +1088,10 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b/>
+      <sz val="44"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue Thin"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1183,7 +1220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1272,21 +1309,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1318,192 +1340,276 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1806,21 +1912,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="41" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" style="36" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="1" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="26.5703125" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" style="43" customWidth="1"/>
-    <col min="6" max="6" width="46.85546875" style="43" customWidth="1"/>
-    <col min="7" max="7" width="37.7109375" style="43" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="38" customWidth="1"/>
+    <col min="6" max="6" width="46.85546875" style="38" customWidth="1"/>
+    <col min="7" max="7" width="37.7109375" style="38" customWidth="1"/>
     <col min="8" max="8" width="21.5703125" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="21.85546875" style="1" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="26.42578125" style="1" hidden="1" customWidth="1"/>
@@ -1829,29 +1935,29 @@
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
+    <row r="1" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-    </row>
-    <row r="2" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-    </row>
-    <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+    </row>
+    <row r="2" spans="1:12" ht="25.5" customHeight="1">
+      <c r="A2" s="71" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+    </row>
+    <row r="3" spans="1:12" ht="45" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1889,14 +1995,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="78" t="s">
+    <row r="4" spans="1:12" ht="72.75" customHeight="1">
+      <c r="A4" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="96" t="s">
+      <c r="C4" s="76" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1915,60 +2021,60 @@
         <v>21</v>
       </c>
       <c r="I4" s="7"/>
-      <c r="J4" s="88" t="s">
+      <c r="J4" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="88" t="s">
+      <c r="K4" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="88" t="s">
+      <c r="L4" s="81" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="79"/>
-      <c r="B5" s="95"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="61" t="s">
+    <row r="5" spans="1:12" ht="51" customHeight="1">
+      <c r="A5" s="73"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="96" t="s">
+      <c r="E5" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="96" t="s">
-        <v>154</v>
-      </c>
-      <c r="G5" s="61" t="s">
-        <v>155</v>
-      </c>
-      <c r="H5" s="107" t="s">
+      <c r="F5" s="76" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="78" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="84" t="s">
         <v>26</v>
       </c>
       <c r="I5" s="8"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="89"/>
-    </row>
-    <row r="6" spans="1:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="79"/>
-      <c r="B6" s="95"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="107"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="82"/>
+    </row>
+    <row r="6" spans="1:12" ht="10.5" customHeight="1">
+      <c r="A6" s="73"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="84"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-    </row>
-    <row r="7" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="79"/>
-      <c r="B7" s="115" t="s">
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
+      <c r="L6" s="83"/>
+    </row>
+    <row r="7" spans="1:12" ht="31.5" customHeight="1">
+      <c r="A7" s="73"/>
+      <c r="B7" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="78" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1978,381 +2084,383 @@
         <v>30</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="H7" s="9" t="s">
+      <c r="I7" s="10"/>
+      <c r="J7" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="88" t="s">
+      <c r="K7" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="88" t="s">
+      <c r="L7" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="L7" s="88" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="79"/>
-      <c r="B8" s="95"/>
-      <c r="C8" s="84"/>
+    </row>
+    <row r="8" spans="1:12" ht="30" customHeight="1">
+      <c r="A8" s="73"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="79"/>
       <c r="D8" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="82"/>
+    </row>
+    <row r="9" spans="1:12" ht="48" customHeight="1">
+      <c r="A9" s="74"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="G8" s="16" t="s">
+      <c r="E9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="83"/>
+      <c r="K9" s="95"/>
+      <c r="L9" s="83"/>
+    </row>
+    <row r="10" spans="1:12" s="14" customFormat="1" ht="45.75" customHeight="1">
+      <c r="A10" s="85" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="88" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="88" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="89"/>
-      <c r="K8" s="108"/>
-      <c r="L8" s="89"/>
-    </row>
-    <row r="9" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="80"/>
-      <c r="B9" s="95"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="H10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="91" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="91" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" s="91" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="14" customFormat="1" ht="42" customHeight="1">
+      <c r="A11" s="86"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" s="92"/>
+      <c r="K11" s="92"/>
+      <c r="L11" s="92"/>
+    </row>
+    <row r="12" spans="1:12" s="14" customFormat="1" ht="36.75" customHeight="1">
+      <c r="A12" s="87"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G12" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="109"/>
-      <c r="L9" s="90"/>
-    </row>
-    <row r="10" spans="1:12" s="14" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="91" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="110" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="110" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="33" t="s">
+      <c r="H12" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="13"/>
+      <c r="J12" s="93"/>
+      <c r="K12" s="93"/>
+      <c r="L12" s="93"/>
+    </row>
+    <row r="13" spans="1:12" s="44" customFormat="1" ht="45.75" customHeight="1">
+      <c r="A13" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="75" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="76"/>
+      <c r="E13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="66" t="s">
-        <v>46</v>
-      </c>
-      <c r="K10" s="66" t="s">
-        <v>47</v>
-      </c>
-      <c r="L10" s="66" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="14" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="92"/>
-      <c r="B11" s="111"/>
-      <c r="C11" s="111"/>
-      <c r="D11" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="12" t="s">
+      <c r="G13" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+    </row>
+    <row r="14" spans="1:12" s="44" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A14" s="74"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
-    </row>
-    <row r="12" spans="1:12" s="14" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="93"/>
-      <c r="B12" s="112"/>
-      <c r="C12" s="112"/>
-      <c r="D12" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="G12" s="44" t="s">
+      <c r="F14" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="H12" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="68"/>
-      <c r="L12" s="68"/>
-    </row>
-    <row r="13" spans="1:12" s="49" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="78" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="95" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="95" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="96"/>
-      <c r="E13" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G13" s="45" t="s">
-        <v>162</v>
-      </c>
-      <c r="H13" s="46" t="s">
+      <c r="G14" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="H14" s="115" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
-    </row>
-    <row r="14" spans="1:12" s="49" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="80"/>
-      <c r="B14" s="95"/>
-      <c r="C14" s="95"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="G14" s="5" t="s">
+      <c r="I14" s="115" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="115" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" s="96" t="s">
+        <v>63</v>
+      </c>
+      <c r="L14" s="96" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="19" customFormat="1" ht="48.75" customHeight="1">
+      <c r="A15" s="85" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="111" t="s">
+        <v>220</v>
+      </c>
+      <c r="C15" s="99" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="F15" s="69" t="s">
+        <v>188</v>
+      </c>
+      <c r="G15" s="69" t="s">
+        <v>187</v>
+      </c>
+      <c r="H15" s="115"/>
+      <c r="I15" s="115"/>
+      <c r="J15" s="115"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+    </row>
+    <row r="16" spans="1:12" s="19" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A16" s="86"/>
+      <c r="B16" s="112"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="84"/>
+      <c r="E16" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="H14" s="103" t="s">
-        <v>61</v>
-      </c>
-      <c r="I14" s="103" t="s">
-        <v>62</v>
-      </c>
-      <c r="J14" s="103" t="s">
-        <v>63</v>
-      </c>
-      <c r="K14" s="104" t="s">
-        <v>64</v>
-      </c>
-      <c r="L14" s="104" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="19" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="91" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="63" t="s">
+      <c r="F16" s="57" t="s">
+        <v>194</v>
+      </c>
+      <c r="G16" s="57" t="s">
+        <v>221</v>
+      </c>
+      <c r="H16" s="115"/>
+      <c r="I16" s="115"/>
+      <c r="J16" s="115"/>
+      <c r="K16" s="98"/>
+      <c r="L16" s="98"/>
+    </row>
+    <row r="17" spans="1:12" s="19" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A17" s="86"/>
+      <c r="B17" s="113"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="52" t="s">
+        <v>190</v>
+      </c>
+      <c r="F17" s="69" t="s">
+        <v>191</v>
+      </c>
+      <c r="G17" s="116" t="s">
         <v>193</v>
       </c>
-      <c r="C15" s="94" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="107" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="H15" s="103"/>
-      <c r="I15" s="103"/>
-      <c r="J15" s="103"/>
-      <c r="K15" s="105"/>
-      <c r="L15" s="105"/>
-    </row>
-    <row r="16" spans="1:12" s="19" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="92"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="94"/>
-      <c r="D16" s="107"/>
-      <c r="E16" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="F16" s="58" t="s">
-        <v>199</v>
-      </c>
-      <c r="G16" s="54"/>
-      <c r="H16" s="103"/>
-      <c r="I16" s="103"/>
-      <c r="J16" s="103"/>
-      <c r="K16" s="106"/>
-      <c r="L16" s="106"/>
-    </row>
-    <row r="17" spans="1:12" s="19" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="92"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="59" t="s">
-        <v>195</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="G17" s="60" t="s">
-        <v>198</v>
-      </c>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
-    </row>
-    <row r="18" spans="1:12" s="19" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="93"/>
-      <c r="B18" s="55" t="s">
-        <v>206</v>
-      </c>
-      <c r="C18" s="53"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+    </row>
+    <row r="18" spans="1:12" s="19" customFormat="1" ht="72.75" customHeight="1">
+      <c r="A18" s="87"/>
+      <c r="B18" s="49" t="s">
+        <v>222</v>
+      </c>
+      <c r="C18" s="48"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G18" s="12"/>
-      <c r="H18" s="97"/>
-      <c r="I18" s="97"/>
-      <c r="J18" s="97"/>
-      <c r="K18" s="98"/>
-      <c r="L18" s="98"/>
-    </row>
-    <row r="19" spans="1:12" s="49" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="99" t="s">
+      <c r="H18" s="100"/>
+      <c r="I18" s="100"/>
+      <c r="J18" s="100"/>
+      <c r="K18" s="114"/>
+      <c r="L18" s="114"/>
+    </row>
+    <row r="19" spans="1:12" s="44" customFormat="1" ht="42" customHeight="1">
+      <c r="A19" s="101" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="100" t="s">
+      <c r="C19" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="95" t="s">
+      <c r="D19" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="96" t="s">
+      <c r="E19" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="61" t="s">
+      <c r="F19" s="78" t="s">
+        <v>168</v>
+      </c>
+      <c r="G19" s="78" t="s">
+        <v>169</v>
+      </c>
+      <c r="H19" s="100"/>
+      <c r="I19" s="100"/>
+      <c r="J19" s="100"/>
+      <c r="K19" s="114"/>
+      <c r="L19" s="114"/>
+    </row>
+    <row r="20" spans="1:12" s="44" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A20" s="101"/>
+      <c r="B20" s="103"/>
+      <c r="C20" s="75"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="100"/>
+      <c r="I20" s="100"/>
+      <c r="J20" s="100"/>
+      <c r="K20" s="114"/>
+      <c r="L20" s="114"/>
+    </row>
+    <row r="21" spans="1:12" s="44" customFormat="1" ht="43.5" customHeight="1">
+      <c r="A21" s="101"/>
+      <c r="B21" s="103"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+    </row>
+    <row r="22" spans="1:12" s="47" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A22" s="101"/>
+      <c r="B22" s="104"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F19" s="61" t="s">
-        <v>171</v>
-      </c>
-      <c r="G19" s="61" t="s">
-        <v>172</v>
-      </c>
-      <c r="H19" s="97"/>
-      <c r="I19" s="97"/>
-      <c r="J19" s="97"/>
-      <c r="K19" s="98"/>
-      <c r="L19" s="98"/>
-    </row>
-    <row r="20" spans="1:12" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="99"/>
-      <c r="B20" s="101"/>
-      <c r="C20" s="95"/>
-      <c r="D20" s="96"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="97"/>
-      <c r="I20" s="97"/>
-      <c r="J20" s="97"/>
-      <c r="K20" s="98"/>
-      <c r="L20" s="98"/>
-    </row>
-    <row r="21" spans="1:12" s="49" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="99"/>
-      <c r="B21" s="101"/>
-      <c r="C21" s="95"/>
-      <c r="D21" s="96"/>
-      <c r="E21" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-    </row>
-    <row r="22" spans="1:12" s="52" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="99"/>
-      <c r="B22" s="102"/>
-      <c r="C22" s="95"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:12" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="A23" s="20"/>
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
@@ -2361,7 +2469,7 @@
       <c r="F23" s="23"/>
       <c r="G23" s="23"/>
     </row>
-    <row r="24" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="45" customHeight="1">
       <c r="A24" s="25" t="s">
         <v>2</v>
       </c>
@@ -2372,635 +2480,662 @@
         <v>4</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>6</v>
       </c>
       <c r="F24" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="G24" s="25" t="s">
+    </row>
+    <row r="25" spans="1:12" ht="27" customHeight="1">
+      <c r="A25" s="72" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="78" t="s">
+      <c r="B25" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="95" t="s">
+      <c r="C25" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="96" t="s">
+      <c r="D25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="H25" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="G25" s="61" t="s">
-        <v>222</v>
-      </c>
-      <c r="H25" s="26" t="s">
+      <c r="I25" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="I25" s="27" t="s">
+      <c r="J25" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="J25" s="88" t="s">
+      <c r="K25" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="K25" s="88" t="s">
+      <c r="L25" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="L25" s="88" t="s">
+    </row>
+    <row r="26" spans="1:12" ht="29.25" customHeight="1">
+      <c r="A26" s="73"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="79"/>
-      <c r="B26" s="95"/>
-      <c r="C26" s="96"/>
-      <c r="D26" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G26" s="79"/>
+      <c r="H26" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="G26" s="84"/>
-      <c r="H26" s="28" t="s">
+      <c r="I26" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="I26" s="18" t="s">
+      <c r="J26" s="82"/>
+      <c r="K26" s="82"/>
+      <c r="L26" s="82"/>
+    </row>
+    <row r="27" spans="1:12" ht="30" customHeight="1">
+      <c r="A27" s="73"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J26" s="89"/>
-      <c r="K26" s="89"/>
-      <c r="L26" s="89"/>
-    </row>
-    <row r="27" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="79"/>
-      <c r="B27" s="95"/>
-      <c r="C27" s="96"/>
-      <c r="D27" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="G27" s="80"/>
+      <c r="H27" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="G27" s="62"/>
-      <c r="H27" s="28" t="s">
+      <c r="I27" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="I27" s="18" t="s">
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="82"/>
+    </row>
+    <row r="28" spans="1:12" ht="57.75" customHeight="1">
+      <c r="A28" s="73"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="J27" s="89"/>
-      <c r="K27" s="89"/>
-      <c r="L27" s="89"/>
-    </row>
-    <row r="28" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="79"/>
-      <c r="B28" s="95"/>
-      <c r="C28" s="96"/>
-      <c r="D28" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="5" t="s">
+      <c r="F28" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="I28" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="H28" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="I28" s="29" t="s">
+      <c r="J28" s="82"/>
+      <c r="K28" s="82"/>
+      <c r="L28" s="82"/>
+    </row>
+    <row r="29" spans="1:12" ht="48" customHeight="1">
+      <c r="A29" s="73"/>
+      <c r="B29" s="75"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="J28" s="89"/>
-      <c r="K28" s="89"/>
-      <c r="L28" s="89"/>
-    </row>
-    <row r="29" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="79"/>
-      <c r="B29" s="95"/>
-      <c r="C29" s="96"/>
-      <c r="D29" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="H29" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="G29" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="H29" s="29" t="s">
+      <c r="I29" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="I29" s="18" t="s">
+      <c r="J29" s="82"/>
+      <c r="K29" s="82"/>
+      <c r="L29" s="82"/>
+    </row>
+    <row r="30" spans="1:12" ht="33" customHeight="1">
+      <c r="A30" s="73"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="J29" s="89"/>
-      <c r="K29" s="89"/>
-      <c r="L29" s="89"/>
-    </row>
-    <row r="30" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="79"/>
-      <c r="B30" s="95"/>
-      <c r="C30" s="96"/>
-      <c r="D30" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" s="5" t="s">
+      <c r="F30" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="I30" s="18"/>
+      <c r="J30" s="82"/>
+      <c r="K30" s="82"/>
+      <c r="L30" s="82"/>
+    </row>
+    <row r="31" spans="1:12" ht="34.5" customHeight="1">
+      <c r="A31" s="74"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="H30" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="89"/>
-      <c r="K30" s="89"/>
-      <c r="L30" s="89"/>
-    </row>
-    <row r="31" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="80"/>
-      <c r="B31" s="95"/>
-      <c r="C31" s="96"/>
-      <c r="D31" s="5" t="s">
+      <c r="E31" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="F31" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="G31" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="H31" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="G31" s="45" t="s">
-        <v>201</v>
-      </c>
-      <c r="H31" s="18" t="s">
+      <c r="I31" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="I31" s="18" t="s">
+      <c r="J31" s="83"/>
+      <c r="K31" s="83"/>
+      <c r="L31" s="83"/>
+    </row>
+    <row r="32" spans="1:12" s="14" customFormat="1" ht="35.25" customHeight="1">
+      <c r="A32" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="J31" s="90"/>
-      <c r="K31" s="90"/>
-      <c r="L31" s="90"/>
-    </row>
-    <row r="32" spans="1:12" s="14" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="91" t="s">
+      <c r="B32" s="99" t="s">
+        <v>174</v>
+      </c>
+      <c r="C32" s="99" t="s">
         <v>105</v>
       </c>
-      <c r="B32" s="94" t="s">
-        <v>177</v>
-      </c>
-      <c r="C32" s="94" t="s">
+      <c r="D32" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="E32" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F32" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="G32" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="I32" s="30"/>
+      <c r="J32" s="91" t="s">
+        <v>109</v>
+      </c>
+      <c r="K32" s="91" t="s">
+        <v>110</v>
+      </c>
+      <c r="L32" s="91" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="14" customFormat="1" ht="53.25" customHeight="1">
+      <c r="A33" s="86"/>
+      <c r="B33" s="99"/>
+      <c r="C33" s="99"/>
+      <c r="D33" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F33" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="F32" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="G32" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="I32" s="30"/>
-      <c r="J32" s="66" t="s">
-        <v>110</v>
-      </c>
-      <c r="K32" s="66" t="s">
-        <v>111</v>
-      </c>
-      <c r="L32" s="66" t="s">
+      <c r="G33" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="H33" s="9" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" s="14" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="92"/>
-      <c r="B33" s="94"/>
-      <c r="C33" s="94"/>
-      <c r="D33" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="H33" s="9" t="s">
+      <c r="I33" s="30"/>
+      <c r="J33" s="93"/>
+      <c r="K33" s="93"/>
+      <c r="L33" s="93"/>
+    </row>
+    <row r="34" spans="1:12" s="14" customFormat="1" ht="65.25" customHeight="1">
+      <c r="A34" s="86"/>
+      <c r="B34" s="99" t="s">
+        <v>219</v>
+      </c>
+      <c r="C34" s="105" t="s">
         <v>113</v>
       </c>
-      <c r="I33" s="30"/>
-      <c r="J33" s="68"/>
-      <c r="K33" s="68"/>
-      <c r="L33" s="68"/>
-    </row>
-    <row r="34" spans="1:12" s="14" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="92"/>
-      <c r="B34" s="94" t="s">
+      <c r="D34" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C34" s="85" t="s">
+      <c r="F34" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="G34" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="H34" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D34" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E34" s="9" t="s">
+      <c r="I34" s="30"/>
+      <c r="J34" s="91" t="s">
         <v>116</v>
       </c>
-      <c r="F34" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="G34" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="H34" s="9" t="s">
+      <c r="K34" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="I34" s="30"/>
-      <c r="J34" s="66" t="s">
+      <c r="L34" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="K34" s="32" t="s">
+    </row>
+    <row r="35" spans="1:12" s="14" customFormat="1" ht="40.5" customHeight="1">
+      <c r="A35" s="86"/>
+      <c r="B35" s="99"/>
+      <c r="C35" s="106"/>
+      <c r="D35" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H35" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="L34" s="32" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="14" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="92"/>
-      <c r="B35" s="94"/>
-      <c r="C35" s="86"/>
-      <c r="D35" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>121</v>
-      </c>
       <c r="I35" s="30"/>
-      <c r="J35" s="67"/>
+      <c r="J35" s="92"/>
       <c r="K35" s="17"/>
       <c r="L35" s="17"/>
     </row>
-    <row r="36" spans="1:12" s="14" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="92"/>
-      <c r="B36" s="94"/>
-      <c r="C36" s="86"/>
+    <row r="36" spans="1:12" s="14" customFormat="1" ht="60.75" customHeight="1">
+      <c r="A36" s="86"/>
+      <c r="B36" s="99"/>
+      <c r="C36" s="106"/>
       <c r="D36" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E36" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="H36" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F36" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>124</v>
-      </c>
       <c r="I36" s="30"/>
-      <c r="J36" s="67"/>
+      <c r="J36" s="92"/>
       <c r="K36" s="17"/>
       <c r="L36" s="17"/>
     </row>
-    <row r="37" spans="1:12" s="14" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="92"/>
-      <c r="B37" s="94"/>
-      <c r="C37" s="86"/>
+    <row r="37" spans="1:12" s="14" customFormat="1" ht="75" customHeight="1">
+      <c r="A37" s="86"/>
+      <c r="B37" s="99"/>
+      <c r="C37" s="106"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="30"/>
-      <c r="J37" s="67"/>
+      <c r="J37" s="92"/>
       <c r="K37" s="17"/>
       <c r="L37" s="17"/>
     </row>
-    <row r="38" spans="1:12" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="92"/>
-      <c r="B38" s="94"/>
-      <c r="C38" s="86"/>
+    <row r="38" spans="1:12" s="14" customFormat="1" ht="50.25" customHeight="1">
+      <c r="A38" s="86"/>
+      <c r="B38" s="99"/>
+      <c r="C38" s="106"/>
       <c r="D38" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F38" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="G38" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="H38" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="G38" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>129</v>
-      </c>
       <c r="I38" s="30"/>
-      <c r="J38" s="67"/>
+      <c r="J38" s="92"/>
       <c r="K38" s="17"/>
       <c r="L38" s="17"/>
     </row>
-    <row r="39" spans="1:12" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="92"/>
-      <c r="B39" s="94"/>
-      <c r="C39" s="86"/>
+    <row r="39" spans="1:12" s="14" customFormat="1" ht="50.25" customHeight="1">
+      <c r="A39" s="86"/>
+      <c r="B39" s="99"/>
+      <c r="C39" s="106"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="30"/>
-      <c r="J39" s="67"/>
+      <c r="J39" s="92"/>
       <c r="K39" s="17"/>
       <c r="L39" s="17"/>
     </row>
-    <row r="40" spans="1:12" s="14" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="92"/>
-      <c r="B40" s="94"/>
-      <c r="C40" s="86"/>
+    <row r="40" spans="1:12" s="14" customFormat="1" ht="36" customHeight="1">
+      <c r="A40" s="86"/>
+      <c r="B40" s="99"/>
+      <c r="C40" s="106"/>
       <c r="D40" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I40" s="30"/>
-      <c r="J40" s="67"/>
+      <c r="J40" s="92"/>
       <c r="K40" s="17"/>
       <c r="L40" s="17"/>
     </row>
-    <row r="41" spans="1:12" s="14" customFormat="1" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="93"/>
-      <c r="B41" s="94"/>
-      <c r="C41" s="87"/>
+    <row r="41" spans="1:12" s="14" customFormat="1" ht="34.5" hidden="1" customHeight="1">
+      <c r="A41" s="87"/>
+      <c r="B41" s="99"/>
+      <c r="C41" s="107"/>
       <c r="D41" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G41" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="H41" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="I41" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="F41" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="G41" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="H41" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="I41" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="J41" s="68"/>
+      <c r="J41" s="93"/>
       <c r="K41" s="34"/>
       <c r="L41" s="34"/>
     </row>
-    <row r="42" spans="1:12" s="14" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="78" t="s">
+    <row r="42" spans="1:12" s="14" customFormat="1" ht="69.75" customHeight="1">
+      <c r="A42" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="B42" s="108" t="s">
+        <v>135</v>
+      </c>
+      <c r="C42" s="78" t="s">
         <v>136</v>
       </c>
-      <c r="B42" s="81" t="s">
+      <c r="D42" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C42" s="61" t="s">
+      <c r="F42" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="H42" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E42" s="4" t="s">
+      <c r="I42" s="105" t="s">
         <v>139</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="H42" s="12" t="s">
+      <c r="J42" s="91" t="s">
         <v>140</v>
       </c>
-      <c r="I42" s="85" t="s">
+      <c r="K42" s="91" t="s">
         <v>141</v>
       </c>
-      <c r="J42" s="66" t="s">
+      <c r="L42" s="91" t="s">
         <v>142</v>
       </c>
-      <c r="K42" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="L42" s="66" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" s="14" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="79"/>
-      <c r="B43" s="82"/>
-      <c r="C43" s="84"/>
+    </row>
+    <row r="43" spans="1:12" s="14" customFormat="1" ht="48.75" customHeight="1">
+      <c r="A43" s="73"/>
+      <c r="B43" s="109"/>
+      <c r="C43" s="79"/>
       <c r="D43" s="5" t="s">
         <v>29</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F43" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="H43" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="I43" s="106"/>
+      <c r="J43" s="92"/>
+      <c r="K43" s="92"/>
+      <c r="L43" s="92"/>
+    </row>
+    <row r="44" spans="1:12" s="35" customFormat="1" ht="101.25" customHeight="1">
+      <c r="A44" s="74"/>
+      <c r="B44" s="110"/>
+      <c r="C44" s="80"/>
+      <c r="D44" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="G44" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="H44" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="I44" s="107"/>
+      <c r="J44" s="93"/>
+      <c r="K44" s="93"/>
+      <c r="L44" s="93"/>
+    </row>
+    <row r="45" spans="1:12" s="119" customFormat="1" ht="101.25" customHeight="1">
+      <c r="A45" s="62" t="s">
+        <v>223</v>
+      </c>
+      <c r="B45" s="120" t="s">
+        <v>224</v>
+      </c>
+      <c r="C45" s="58"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="121" t="s">
+        <v>137</v>
+      </c>
+      <c r="F45" s="69" t="s">
+        <v>209</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="118"/>
+      <c r="K45" s="118"/>
+      <c r="L45" s="118"/>
+    </row>
+    <row r="46" spans="1:12" ht="34.5" customHeight="1">
+      <c r="A46" s="72" t="s">
+        <v>146</v>
+      </c>
+      <c r="B46" s="108" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46" s="108" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" s="122"/>
+      <c r="E46" s="78" t="s">
+        <v>149</v>
+      </c>
+      <c r="F46" s="66" t="s">
+        <v>180</v>
+      </c>
+      <c r="G46" s="117" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="34.5" customHeight="1">
+      <c r="A47" s="73"/>
+      <c r="B47" s="110"/>
+      <c r="C47" s="110"/>
+      <c r="D47" s="123"/>
+      <c r="E47" s="80"/>
+      <c r="F47" s="66" t="s">
+        <v>181</v>
+      </c>
+      <c r="G47" s="117" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="48" customHeight="1">
+      <c r="A48" s="74"/>
+      <c r="B48" s="124" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="D48" s="125"/>
+      <c r="E48" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="F48" s="66" t="s">
         <v>182</v>
       </c>
-      <c r="G43" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="H43" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="I43" s="86"/>
-      <c r="J43" s="67"/>
-      <c r="K43" s="67"/>
-      <c r="L43" s="67"/>
-    </row>
-    <row r="44" spans="1:12" s="35" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="80"/>
-      <c r="B44" s="83"/>
-      <c r="C44" s="62"/>
-      <c r="D44" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="G44" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="H44" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="I44" s="87"/>
-      <c r="J44" s="68"/>
-      <c r="K44" s="68"/>
-      <c r="L44" s="68"/>
-    </row>
-    <row r="45" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="69" t="s">
-        <v>148</v>
-      </c>
-      <c r="B45" s="72" t="s">
-        <v>149</v>
-      </c>
-      <c r="C45" s="72" t="s">
-        <v>150</v>
-      </c>
-      <c r="D45" s="74"/>
-      <c r="E45" s="76" t="s">
-        <v>151</v>
-      </c>
-      <c r="F45" s="18" t="s">
+      <c r="G48" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="G45" s="36" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="70"/>
-      <c r="B46" s="73"/>
-      <c r="C46" s="73"/>
-      <c r="D46" s="75"/>
-      <c r="E46" s="77"/>
-      <c r="F46" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="G46" s="36" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="71"/>
-      <c r="B47" s="37" t="s">
-        <v>152</v>
-      </c>
-      <c r="C47" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="D47" s="39"/>
-      <c r="E47" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="F47" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="G47" s="40" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B48" s="42"/>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="K10:K12"/>
-    <mergeCell ref="L10:L12"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="K14:K16"/>
+    <mergeCell ref="L18:L20"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="L42:L44"/>
+    <mergeCell ref="K42:K44"/>
+    <mergeCell ref="L25:L31"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="K25:K31"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="I42:I44"/>
+    <mergeCell ref="J42:J44"/>
+    <mergeCell ref="A32:A41"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="B34:B41"/>
+    <mergeCell ref="C34:C41"/>
+    <mergeCell ref="J34:J41"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="C25:C31"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="J25:J31"/>
     <mergeCell ref="L14:L16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D15:D16"/>
@@ -3010,62 +3145,1032 @@
     <mergeCell ref="C19:C22"/>
     <mergeCell ref="D19:D22"/>
     <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="C25:C31"/>
-    <mergeCell ref="G25:G27"/>
-    <mergeCell ref="J25:J31"/>
-    <mergeCell ref="A32:A41"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="B34:B41"/>
-    <mergeCell ref="C34:C41"/>
-    <mergeCell ref="J34:J41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="I42:I44"/>
-    <mergeCell ref="J42:J44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="B15:B17"/>
-    <mergeCell ref="L42:L44"/>
-    <mergeCell ref="K42:K44"/>
-    <mergeCell ref="L25:L31"/>
-    <mergeCell ref="L32:L33"/>
-    <mergeCell ref="K25:K31"/>
     <mergeCell ref="I18:I20"/>
     <mergeCell ref="J18:J20"/>
     <mergeCell ref="K18:K20"/>
-    <mergeCell ref="L18:L20"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="K14:K16"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="L10:L12"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G17" r:id="rId1" display="http://dlnr.hawaii.gov/occl/conservation-district/; geodata.portal"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" verticalDpi="360" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G46" sqref="A3:G46"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <cols>
+    <col min="1" max="2" width="7.85546875" style="139" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="14" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" style="14" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" style="120" customWidth="1"/>
+    <col min="7" max="7" width="46.85546875" style="120" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="3.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A1" s="126" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+    </row>
+    <row r="2" spans="1:12" ht="44.25" customHeight="1">
+      <c r="A2" s="127" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
+    </row>
+    <row r="3" spans="1:12" ht="45" customHeight="1">
+      <c r="A3" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="72.75" customHeight="1">
+      <c r="A4" s="85" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="61"/>
+      <c r="C4" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="69" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="60" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="31.5" customHeight="1">
+      <c r="A5" s="86"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="128" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="105" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="129"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="81" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="81" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="81" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" customHeight="1">
+      <c r="A6" s="86"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="106"/>
+      <c r="E6" s="130" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="69"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="82"/>
+    </row>
+    <row r="7" spans="1:12" ht="48" customHeight="1">
+      <c r="A7" s="87"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="69"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="83"/>
+    </row>
+    <row r="8" spans="1:12" s="14" customFormat="1" ht="45.75" customHeight="1">
+      <c r="A8" s="85" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="61"/>
+      <c r="C8" s="88" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="88" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="13"/>
+      <c r="J8" s="91" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="91" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="91" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="14" customFormat="1" ht="42" customHeight="1">
+      <c r="A9" s="86"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="92"/>
+      <c r="K9" s="92"/>
+      <c r="L9" s="92"/>
+    </row>
+    <row r="10" spans="1:12" s="14" customFormat="1" ht="36.75" customHeight="1">
+      <c r="A10" s="87"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="69"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="93"/>
+      <c r="K10" s="93"/>
+      <c r="L10" s="93"/>
+    </row>
+    <row r="11" spans="1:12" s="44" customFormat="1" ht="45.75" customHeight="1">
+      <c r="A11" s="85" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="61"/>
+      <c r="C11" s="99" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="99" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="84"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+    </row>
+    <row r="12" spans="1:12" s="44" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A12" s="87"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="99"/>
+      <c r="D12" s="99"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="115" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="115" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="115" t="s">
+        <v>62</v>
+      </c>
+      <c r="K12" s="96" t="s">
+        <v>63</v>
+      </c>
+      <c r="L12" s="96" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="19" customFormat="1" ht="48.75" customHeight="1">
+      <c r="A13" s="85" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="61"/>
+      <c r="C13" s="111" t="s">
+        <v>220</v>
+      </c>
+      <c r="D13" s="99" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="115"/>
+      <c r="I13" s="115"/>
+      <c r="J13" s="115"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="97"/>
+    </row>
+    <row r="14" spans="1:12" s="19" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A14" s="86"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="112"/>
+      <c r="D14" s="99"/>
+      <c r="E14" s="84"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="115"/>
+      <c r="I14" s="115"/>
+      <c r="J14" s="115"/>
+      <c r="K14" s="98"/>
+      <c r="L14" s="98"/>
+    </row>
+    <row r="15" spans="1:12" s="19" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A15" s="86"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="113"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="68"/>
+    </row>
+    <row r="16" spans="1:12" s="19" customFormat="1" ht="72.75" customHeight="1">
+      <c r="A16" s="87"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="49" t="s">
+        <v>222</v>
+      </c>
+      <c r="D16" s="64"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="100"/>
+      <c r="I16" s="100"/>
+      <c r="J16" s="100"/>
+      <c r="K16" s="114"/>
+      <c r="L16" s="114"/>
+    </row>
+    <row r="17" spans="1:12" s="44" customFormat="1" ht="42" customHeight="1">
+      <c r="A17" s="131" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="61"/>
+      <c r="C17" s="132" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="84" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="105"/>
+      <c r="G17" s="105"/>
+      <c r="H17" s="100"/>
+      <c r="I17" s="100"/>
+      <c r="J17" s="100"/>
+      <c r="K17" s="114"/>
+      <c r="L17" s="114"/>
+    </row>
+    <row r="18" spans="1:12" s="44" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A18" s="131"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="133"/>
+      <c r="D18" s="99"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="107"/>
+      <c r="G18" s="107"/>
+      <c r="H18" s="100"/>
+      <c r="I18" s="100"/>
+      <c r="J18" s="100"/>
+      <c r="K18" s="114"/>
+      <c r="L18" s="114"/>
+    </row>
+    <row r="19" spans="1:12" s="44" customFormat="1" ht="43.5" customHeight="1">
+      <c r="A19" s="131"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="133"/>
+      <c r="D19" s="99"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+    </row>
+    <row r="20" spans="1:12" s="47" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A20" s="131"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="134"/>
+      <c r="D20" s="99"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
+    </row>
+    <row r="21" spans="1:12" s="24" customFormat="1" ht="12" customHeight="1">
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+    </row>
+    <row r="22" spans="1:12" ht="45" customHeight="1">
+      <c r="A22" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+    </row>
+    <row r="23" spans="1:12" ht="27" customHeight="1">
+      <c r="A23" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="61"/>
+      <c r="C23" s="99" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="84" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="I23" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="J23" s="81" t="s">
+        <v>84</v>
+      </c>
+      <c r="K23" s="81" t="s">
+        <v>85</v>
+      </c>
+      <c r="L23" s="81" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="29.25" customHeight="1">
+      <c r="A24" s="86"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="99"/>
+      <c r="D24" s="84"/>
+      <c r="E24" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="J24" s="82"/>
+      <c r="K24" s="82"/>
+      <c r="L24" s="82"/>
+    </row>
+    <row r="25" spans="1:12" ht="30" customHeight="1">
+      <c r="A25" s="86"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="99"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="69"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="I25" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="J25" s="82"/>
+      <c r="K25" s="82"/>
+      <c r="L25" s="82"/>
+    </row>
+    <row r="26" spans="1:12" ht="57.75" customHeight="1">
+      <c r="A26" s="86"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="99"/>
+      <c r="D26" s="84"/>
+      <c r="E26" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="69"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="I26" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="J26" s="82"/>
+      <c r="K26" s="82"/>
+      <c r="L26" s="82"/>
+    </row>
+    <row r="27" spans="1:12" ht="48" customHeight="1">
+      <c r="A27" s="86"/>
+      <c r="B27" s="62"/>
+      <c r="C27" s="99"/>
+      <c r="D27" s="84"/>
+      <c r="E27" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="69"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="82"/>
+    </row>
+    <row r="28" spans="1:12" ht="33" customHeight="1">
+      <c r="A28" s="86"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="99"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="69"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="I28" s="18"/>
+      <c r="J28" s="82"/>
+      <c r="K28" s="82"/>
+      <c r="L28" s="82"/>
+    </row>
+    <row r="29" spans="1:12" ht="34.5" customHeight="1">
+      <c r="A29" s="87"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="99"/>
+      <c r="D29" s="84"/>
+      <c r="E29" s="69" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="J29" s="83"/>
+      <c r="K29" s="83"/>
+      <c r="L29" s="83"/>
+    </row>
+    <row r="30" spans="1:12" s="14" customFormat="1" ht="35.25" customHeight="1">
+      <c r="A30" s="85" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="61"/>
+      <c r="C30" s="99" t="s">
+        <v>174</v>
+      </c>
+      <c r="D30" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="I30" s="30"/>
+      <c r="J30" s="91" t="s">
+        <v>109</v>
+      </c>
+      <c r="K30" s="91" t="s">
+        <v>110</v>
+      </c>
+      <c r="L30" s="91" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="14" customFormat="1" ht="53.25" customHeight="1">
+      <c r="A31" s="86"/>
+      <c r="B31" s="62"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="99"/>
+      <c r="E31" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="I31" s="30"/>
+      <c r="J31" s="93"/>
+      <c r="K31" s="93"/>
+      <c r="L31" s="93"/>
+    </row>
+    <row r="32" spans="1:12" s="14" customFormat="1" ht="65.25" customHeight="1">
+      <c r="A32" s="86"/>
+      <c r="B32" s="62"/>
+      <c r="C32" s="99" t="s">
+        <v>219</v>
+      </c>
+      <c r="D32" s="105" t="s">
+        <v>113</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="I32" s="30"/>
+      <c r="J32" s="91" t="s">
+        <v>116</v>
+      </c>
+      <c r="K32" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="L32" s="53" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="14" customFormat="1" ht="40.5" customHeight="1">
+      <c r="A33" s="86"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="99"/>
+      <c r="D33" s="106"/>
+      <c r="E33" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="I33" s="30"/>
+      <c r="J33" s="92"/>
+      <c r="K33" s="54"/>
+      <c r="L33" s="54"/>
+    </row>
+    <row r="34" spans="1:12" s="14" customFormat="1" ht="60.75" customHeight="1">
+      <c r="A34" s="86"/>
+      <c r="B34" s="62"/>
+      <c r="C34" s="99"/>
+      <c r="D34" s="106"/>
+      <c r="E34" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I34" s="30"/>
+      <c r="J34" s="92"/>
+      <c r="K34" s="54"/>
+      <c r="L34" s="54"/>
+    </row>
+    <row r="35" spans="1:12" s="14" customFormat="1" ht="75" customHeight="1">
+      <c r="A35" s="86"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="99"/>
+      <c r="D35" s="106"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="92"/>
+      <c r="K35" s="54"/>
+      <c r="L35" s="54"/>
+    </row>
+    <row r="36" spans="1:12" s="14" customFormat="1" ht="50.25" customHeight="1">
+      <c r="A36" s="86"/>
+      <c r="B36" s="62"/>
+      <c r="C36" s="99"/>
+      <c r="D36" s="106"/>
+      <c r="E36" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="I36" s="30"/>
+      <c r="J36" s="92"/>
+      <c r="K36" s="54"/>
+      <c r="L36" s="54"/>
+    </row>
+    <row r="37" spans="1:12" s="14" customFormat="1" ht="50.25" customHeight="1">
+      <c r="A37" s="86"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="106"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="92"/>
+      <c r="K37" s="54"/>
+      <c r="L37" s="54"/>
+    </row>
+    <row r="38" spans="1:12" s="14" customFormat="1" ht="36" customHeight="1">
+      <c r="A38" s="86"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="99"/>
+      <c r="D38" s="106"/>
+      <c r="E38" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="I38" s="30"/>
+      <c r="J38" s="92"/>
+      <c r="K38" s="54"/>
+      <c r="L38" s="54"/>
+    </row>
+    <row r="39" spans="1:12" s="14" customFormat="1" ht="34.5" hidden="1" customHeight="1">
+      <c r="A39" s="87"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="99"/>
+      <c r="D39" s="107"/>
+      <c r="E39" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="J39" s="93"/>
+      <c r="K39" s="55"/>
+      <c r="L39" s="55"/>
+    </row>
+    <row r="40" spans="1:12" s="14" customFormat="1" ht="69.75" customHeight="1">
+      <c r="A40" s="85" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" s="61"/>
+      <c r="C40" s="88" t="s">
+        <v>135</v>
+      </c>
+      <c r="D40" s="105" t="s">
+        <v>136</v>
+      </c>
+      <c r="E40" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="F40" s="9"/>
+      <c r="G40" s="69"/>
+      <c r="H40" s="69" t="s">
+        <v>138</v>
+      </c>
+      <c r="I40" s="105" t="s">
+        <v>139</v>
+      </c>
+      <c r="J40" s="91" t="s">
+        <v>140</v>
+      </c>
+      <c r="K40" s="91" t="s">
+        <v>141</v>
+      </c>
+      <c r="L40" s="91" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="14" customFormat="1" ht="48.75" customHeight="1">
+      <c r="A41" s="86"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="106"/>
+      <c r="E41" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="69" t="s">
+        <v>143</v>
+      </c>
+      <c r="I41" s="106"/>
+      <c r="J41" s="92"/>
+      <c r="K41" s="92"/>
+      <c r="L41" s="92"/>
+    </row>
+    <row r="42" spans="1:12" s="35" customFormat="1" ht="101.25" customHeight="1">
+      <c r="A42" s="87"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="90"/>
+      <c r="D42" s="107"/>
+      <c r="E42" s="69" t="s">
+        <v>144</v>
+      </c>
+      <c r="F42" s="9"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="69" t="s">
+        <v>145</v>
+      </c>
+      <c r="I42" s="107"/>
+      <c r="J42" s="93"/>
+      <c r="K42" s="93"/>
+      <c r="L42" s="93"/>
+    </row>
+    <row r="43" spans="1:12" s="119" customFormat="1" ht="101.25" customHeight="1">
+      <c r="A43" s="62" t="s">
+        <v>223</v>
+      </c>
+      <c r="B43" s="20"/>
+      <c r="C43" s="120" t="s">
+        <v>224</v>
+      </c>
+      <c r="D43" s="58"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="121"/>
+      <c r="G43" s="69"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="118"/>
+      <c r="K43" s="118"/>
+      <c r="L43" s="118"/>
+    </row>
+    <row r="44" spans="1:12" s="47" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A44" s="85" t="s">
+        <v>146</v>
+      </c>
+      <c r="B44" s="61"/>
+      <c r="C44" s="88" t="s">
+        <v>147</v>
+      </c>
+      <c r="D44" s="88" t="s">
+        <v>148</v>
+      </c>
+      <c r="E44" s="135"/>
+      <c r="F44" s="105"/>
+      <c r="G44" s="69"/>
+    </row>
+    <row r="45" spans="1:12" s="47" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A45" s="86"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="90"/>
+      <c r="D45" s="90"/>
+      <c r="E45" s="136"/>
+      <c r="F45" s="107"/>
+      <c r="G45" s="69"/>
+    </row>
+    <row r="46" spans="1:12" s="47" customFormat="1" ht="48" customHeight="1">
+      <c r="A46" s="87"/>
+      <c r="B46" s="63"/>
+      <c r="C46" s="137" t="s">
+        <v>150</v>
+      </c>
+      <c r="D46" s="64" t="s">
+        <v>151</v>
+      </c>
+      <c r="E46" s="138"/>
+      <c r="F46" s="69"/>
+      <c r="G46" s="69"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="C47" s="140"/>
+    </row>
+  </sheetData>
+  <mergeCells count="65">
+    <mergeCell ref="L40:L42"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="I40:I42"/>
+    <mergeCell ref="J40:J42"/>
+    <mergeCell ref="K40:K42"/>
+    <mergeCell ref="L23:L29"/>
+    <mergeCell ref="A30:A39"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="C32:C39"/>
+    <mergeCell ref="D32:D39"/>
+    <mergeCell ref="J32:J39"/>
+    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="C23:C29"/>
+    <mergeCell ref="D23:D29"/>
+    <mergeCell ref="J23:J29"/>
+    <mergeCell ref="K23:K29"/>
+    <mergeCell ref="K16:K18"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="L5:L7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="J5:J7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3076,7 +4181,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>